<commit_message>
Some more slight changes to the DFS algorithm, probably giving up on it
</commit_message>
<xml_diff>
--- a/build files and notes/sheet w build methods info.xlsx
+++ b/build files and notes/sheet w build methods info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samo\OneDrive\Documents\C\C2export\build files and notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2E5BAAAB-D67C-49C7-96AF-304AE2FA528D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>0A</t>
   </si>
@@ -267,12 +267,6 @@
     <t>tested, works, no known lags</t>
   </si>
   <si>
-    <t>Rel Occurence matrix (no LL regeneration)</t>
-  </si>
-  <si>
-    <t>Rel. Occurence Matrix (LL regeneration)</t>
-  </si>
-  <si>
     <t>LL Gen. Settings</t>
   </si>
   <si>
@@ -280,6 +274,15 @@
   </si>
   <si>
     <t>Occurence matrix   (no LL regeneration)</t>
+  </si>
+  <si>
+    <t>State Search DFS (LL regeneration)</t>
+  </si>
+  <si>
+    <t>DFS then Payload                (no LL regeneration)</t>
+  </si>
+  <si>
+    <t>no premerge</t>
   </si>
 </sst>
 </file>
@@ -719,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -946,6 +949,30 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1039,28 +1066,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1390,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AD2FBA-18F5-4705-80AA-981EA7CD31DD}">
   <dimension ref="B1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1406,119 +1412,119 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="106"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="114"/>
       <c r="G2" s="55"/>
-      <c r="H2" s="134" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="135"/>
-      <c r="J2" s="136"/>
+      <c r="H2" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="143"/>
+      <c r="J2" s="144"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="115" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="109"/>
-      <c r="H4" s="114" t="s">
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="117"/>
+      <c r="H4" s="122" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="115"/>
-      <c r="J4" s="116"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="124"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="131" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="125"/>
-      <c r="H5" s="117" t="s">
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="133"/>
+      <c r="H5" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="118"/>
-      <c r="J5" s="119"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="134" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="128"/>
-      <c r="H6" s="120" t="s">
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="136"/>
+      <c r="H6" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="121"/>
-      <c r="J6" s="122"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="130"/>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="142" t="s">
+      <c r="B7" s="109" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="144"/>
-      <c r="H7" s="129" t="s">
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="111"/>
+      <c r="H7" s="137" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="131"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="139"/>
     </row>
     <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="140" t="s">
+      <c r="C10" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="140" t="s">
+      <c r="D10" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="110" t="s">
+      <c r="E10" s="118" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="140" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="141"/>
+      <c r="H10" s="118" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="132" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="133"/>
-      <c r="H10" s="110" t="s">
+      <c r="I10" s="120" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="121"/>
+    </row>
+    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="106"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="51" t="s">
         <v>77</v>
-      </c>
-      <c r="I10" s="112" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="113"/>
-    </row>
-    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="139"/>
-      <c r="C11" s="141"/>
-      <c r="D11" s="141"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="51" t="s">
-        <v>79</v>
       </c>
       <c r="G11" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="111"/>
+      <c r="H11" s="119"/>
       <c r="I11" s="68" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J11" s="69" t="s">
         <v>46</v>
@@ -1543,7 +1549,9 @@
       <c r="G12" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="74"/>
+      <c r="H12" s="145" t="s">
+        <v>82</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="65"/>
     </row>
@@ -1602,7 +1610,9 @@
       <c r="G15" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="74"/>
+      <c r="H15" s="145" t="s">
+        <v>82</v>
+      </c>
       <c r="I15" s="78"/>
       <c r="J15" s="76"/>
     </row>
@@ -1659,7 +1669,9 @@
       <c r="G18" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="62"/>
+      <c r="H18" s="86" t="s">
+        <v>82</v>
+      </c>
       <c r="I18" s="2"/>
       <c r="J18" s="65"/>
     </row>
@@ -2037,16 +2049,11 @@
       <c r="J39" s="67"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F40" s="137"/>
-      <c r="G40" s="137"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B7:F7"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H10:H11"/>
@@ -2060,6 +2067,11 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed bug that caused extern GOOL entries' EIDs to be used in NSD. NSD now contains proper DAT_L EID at 0x408.
</commit_message>
<xml_diff>
--- a/build files and notes/sheet w build methods info.xlsx
+++ b/build files and notes/sheet w build methods info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2E5BAAAB-D67C-49C7-96AF-304AE2FA528D}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EC931A79-195B-41C5-A3CA-ED807B66E179}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
+    <workbookView xWindow="13224" yWindow="0" windowWidth="7656" windowHeight="4200" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
   <si>
     <t>0A</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>no premerge</t>
+  </si>
+  <si>
+    <t>both premerges</t>
   </si>
 </sst>
 </file>
@@ -949,6 +952,9 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1064,9 +1070,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1396,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AD2FBA-18F5-4705-80AA-981EA7CD31DD}">
   <dimension ref="B1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1412,117 +1415,117 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="115"/>
       <c r="G2" s="55"/>
-      <c r="H2" s="142" t="s">
+      <c r="H2" s="143" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="143"/>
-      <c r="J2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="145"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="117"/>
-      <c r="H4" s="122" t="s">
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="118"/>
+      <c r="H4" s="123" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="123"/>
-      <c r="J4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="125"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="132" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="133"/>
-      <c r="H5" s="125" t="s">
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="134"/>
+      <c r="H5" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="126"/>
-      <c r="J5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="128"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="134" t="s">
+      <c r="B6" s="135" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="136"/>
-      <c r="H6" s="128" t="s">
+      <c r="C6" s="136"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="137"/>
+      <c r="H6" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="129"/>
-      <c r="J6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="131"/>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="111"/>
-      <c r="H7" s="137" t="s">
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="112"/>
+      <c r="H7" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="138"/>
-      <c r="J7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="140"/>
     </row>
     <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="106" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="107" t="s">
+      <c r="C10" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="107" t="s">
+      <c r="D10" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="118" t="s">
+      <c r="E10" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="140" t="s">
+      <c r="F10" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="141"/>
-      <c r="H10" s="118" t="s">
+      <c r="G10" s="142"/>
+      <c r="H10" s="119" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="120" t="s">
+      <c r="I10" s="121" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="121"/>
+      <c r="J10" s="122"/>
     </row>
     <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="106"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="119"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="120"/>
       <c r="F11" s="51" t="s">
         <v>77</v>
       </c>
       <c r="G11" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="119"/>
+      <c r="H11" s="120"/>
       <c r="I11" s="68" t="s">
         <v>77</v>
       </c>
@@ -1549,7 +1552,7 @@
       <c r="G12" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="145" t="s">
+      <c r="H12" s="104" t="s">
         <v>82</v>
       </c>
       <c r="I12" s="2"/>
@@ -1610,7 +1613,7 @@
       <c r="G15" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="145" t="s">
+      <c r="H15" s="104" t="s">
         <v>82</v>
       </c>
       <c r="I15" s="78"/>
@@ -1711,7 +1714,9 @@
       <c r="G20" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="62"/>
+      <c r="H20" s="86" t="s">
+        <v>83</v>
+      </c>
       <c r="I20" s="2"/>
       <c r="J20" s="65"/>
     </row>
@@ -2049,8 +2054,8 @@
       <c r="J39" s="67"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F40" s="104"/>
-      <c r="G40" s="104"/>
+      <c r="F40" s="105"/>
+      <c r="G40" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>

<commit_message>
state_eval function optimisation, added night fight perma list
</commit_message>
<xml_diff>
--- a/build files and notes/sheet w build methods info.xlsx
+++ b/build files and notes/sheet w build methods info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CED045B7-515D-403D-B938-45CF692D2B91}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0044E48-BB6B-4DB7-8E94-D390E7C5E517}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>0A</t>
   </si>
@@ -183,18 +183,6 @@
     <t>Occurence matrix (LL regeneration)</t>
   </si>
   <si>
-    <t>7000 7000 7000 1 0.5</t>
-  </si>
-  <si>
-    <t>7500 7500 7500 0 .15</t>
-  </si>
-  <si>
-    <t>9000 9000 9000 1 0.0</t>
-  </si>
-  <si>
-    <t>7500 7500 7500 1 0.0</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
@@ -204,24 +192,12 @@
     <t>ID</t>
   </si>
   <si>
-    <t>probably working but not sure, needs testing</t>
-  </si>
-  <si>
-    <t>assumed to be working, testing still recommended</t>
-  </si>
-  <si>
     <t>untested</t>
   </si>
   <si>
     <t>tested, does not work (crashes)</t>
   </si>
   <si>
-    <t>almost definitely crashes, testing probably not necessary</t>
-  </si>
-  <si>
-    <t>likely lags or crashes, testing might prove opposite</t>
-  </si>
-  <si>
     <t>LL Settings format: SLST_DIST NEIG_DIST DRAW_DIST TRNS_PRLD BACK_PENLTY</t>
   </si>
   <si>
@@ -243,27 +219,12 @@
     <t>21, 20, 20, 19, 19</t>
   </si>
   <si>
-    <t>almost definitely works, testing probably not necessary</t>
-  </si>
-  <si>
-    <t>*** Xebra crash (mode 1), works elsewhere</t>
-  </si>
-  <si>
-    <t>&lt;Xebra crash (mode 1), works elsewhere&gt;</t>
-  </si>
-  <si>
-    <t>&lt;18, 16, 16, 16, 16&gt;</t>
-  </si>
-  <si>
     <t>18, 17, 17, 17, 17</t>
   </si>
   <si>
     <t>19, 18, 17, 17, 17</t>
   </si>
   <si>
-    <t>&lt;17, 16, 16, 16, 16&gt;</t>
-  </si>
-  <si>
     <t>int config[] = {</t>
   </si>
   <si>
@@ -313,13 +274,22 @@
   </si>
   <si>
     <t>18, 18, 17, 17, 17</t>
+  </si>
+  <si>
+    <t>18, 16, 16, 16, 16</t>
+  </si>
+  <si>
+    <t>17, 16, 16, 16, 16</t>
+  </si>
+  <si>
+    <t>Xebra crash (mode 1/2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,13 +344,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
@@ -388,7 +351,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,18 +402,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -463,13 +414,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF7979"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -771,7 +722,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -815,12 +765,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -832,255 +782,199 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1091,13 +985,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFCC00CC"/>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFFF99FF"/>
       <color rgb="FFFF7979"/>
       <color rgb="FFFF0000"/>
+      <color rgb="FFCC00CC"/>
       <color rgb="FFFF5757"/>
       <color rgb="FF777777"/>
-      <color rgb="FFFF99FF"/>
-      <color rgb="FFFF6600"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1408,15 +1302,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AD2FBA-18F5-4705-80AA-981EA7CD31DD}">
-  <dimension ref="B1:J41"/>
+  <dimension ref="B1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" customWidth="1"/>
@@ -1427,624 +1321,576 @@
     <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="67" t="s">
+    <row r="1" spans="2:9" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="114" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="116"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="60"/>
+    </row>
+    <row r="4" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="120" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="122"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="83" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="85"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="88"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="91"/>
+    </row>
+    <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="117" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="119"/>
+    </row>
+    <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="95"/>
+      <c r="I11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="80"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="62"/>
+      <c r="G13" s="70"/>
+      <c r="I13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="63"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="71"/>
+      <c r="I14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="98" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="62"/>
+      <c r="G15" s="70"/>
+      <c r="I15" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="112" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="96" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="59"/>
+      <c r="G16" s="72"/>
+      <c r="I16" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="63"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="71"/>
+      <c r="I17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="104" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="56">
+        <v>10</v>
+      </c>
+      <c r="E18" s="63"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="71"/>
+      <c r="I18" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="111" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="36">
+        <v>11</v>
+      </c>
+      <c r="E19" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="110" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="111"/>
-      <c r="J2" s="112"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-    </row>
-    <row r="4" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="107" t="s">
+      <c r="F19" s="47"/>
+      <c r="G19" s="71"/>
+      <c r="I19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="114"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="114"/>
-      <c r="F4" s="115"/>
-      <c r="H4" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="108"/>
-      <c r="J4" s="109"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="116" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="117"/>
-      <c r="H5" s="105" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="104"/>
-      <c r="J5" s="106"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="77" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="79"/>
-      <c r="H6" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="72"/>
-      <c r="J6" s="73"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="80" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="82"/>
-      <c r="H7" s="74" t="s">
+    </row>
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="42">
+        <v>12</v>
+      </c>
+      <c r="E20" s="63"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="71"/>
+      <c r="I20" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="111" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="36">
+        <v>13</v>
+      </c>
+      <c r="E21" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
-    </row>
-    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="93" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
-      <c r="H8" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="84"/>
-      <c r="J8" s="85"/>
-    </row>
-    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="89" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="91" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="118" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="87"/>
-      <c r="I11" s="1" t="s">
+      <c r="F21" s="47"/>
+      <c r="G21" s="71"/>
+      <c r="I21" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="106" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="28">
+        <v>15</v>
+      </c>
+      <c r="E22" s="64"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="71"/>
+      <c r="I22" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="43">
+        <v>16</v>
+      </c>
+      <c r="E23" s="64"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="71"/>
+      <c r="I23" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="106" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="28">
+        <v>17</v>
+      </c>
+      <c r="E24" s="64"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="71"/>
+      <c r="I24" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="90"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="1" t="s">
+    <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="106" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="28">
+        <v>18</v>
+      </c>
+      <c r="E25" s="64"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="71"/>
+      <c r="I25" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="121" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="123"/>
-      <c r="I13" s="1" t="s">
+    <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="113" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="40">
+        <v>19</v>
+      </c>
+      <c r="E26" s="64"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="71"/>
+      <c r="I26" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="97"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="124"/>
-      <c r="I14" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="56" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="122" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="123"/>
-      <c r="I15" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="96" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="125"/>
-      <c r="I16" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="97"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="124"/>
-      <c r="I17" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="59">
-        <v>10</v>
-      </c>
-      <c r="E18" s="97"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="124"/>
-      <c r="I18" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="37">
-        <v>11</v>
-      </c>
-      <c r="E19" s="133" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" s="124"/>
-      <c r="I19" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="18" t="s">
+    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="109" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="43">
-        <v>12</v>
-      </c>
-      <c r="E20" s="97"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="124"/>
-      <c r="I20" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="37">
-        <v>13</v>
-      </c>
-      <c r="E21" s="133" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="124"/>
-      <c r="I21" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="19" t="s">
+      <c r="D27" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="65"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="73"/>
+    </row>
+    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="29">
-        <v>15</v>
-      </c>
-      <c r="E22" s="98"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="124"/>
-      <c r="I22" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="44">
-        <v>16</v>
-      </c>
-      <c r="E23" s="98"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="124"/>
-      <c r="I23" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="29">
-        <v>17</v>
-      </c>
-      <c r="E24" s="98"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="124"/>
-      <c r="I24" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="29">
-        <v>18</v>
-      </c>
-      <c r="E25" s="98"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="124"/>
-      <c r="I25" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="41">
-        <v>19</v>
-      </c>
-      <c r="E26" s="98"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="124"/>
-      <c r="I26" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="99"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="126"/>
-    </row>
-    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="98"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="124"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="71"/>
     </row>
     <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="20" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="101"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="126"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="73"/>
     </row>
     <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="131" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="124"/>
+      <c r="E30" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="47"/>
+      <c r="G30" s="71"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="132" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="65"/>
+      <c r="E31" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="59"/>
+      <c r="G31" s="61"/>
     </row>
     <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="9"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="127"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="74"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="39">
+      <c r="D33" s="38">
         <v>20</v>
       </c>
-      <c r="E33" s="100"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="65"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="61"/>
     </row>
     <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="39">
+      <c r="D34" s="38">
         <v>21</v>
       </c>
-      <c r="E34" s="100"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="65"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="61"/>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="7">
         <v>22</v>
       </c>
-      <c r="E35" s="61"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="128"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="75"/>
     </row>
     <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36" s="27">
         <v>23</v>
       </c>
-      <c r="E36" s="120" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="48"/>
-      <c r="G36" s="129"/>
+      <c r="E36" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="47"/>
+      <c r="G36" s="76"/>
     </row>
     <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="30">
+      <c r="D37" s="29">
         <v>24</v>
       </c>
-      <c r="E37" s="47"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="130"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="77"/>
     </row>
     <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="25" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="4">
         <v>25</v>
       </c>
-      <c r="E38" s="62"/>
-      <c r="F38" s="63"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="36">
+      <c r="D39" s="35">
         <v>26</v>
       </c>
-      <c r="E39" s="47"/>
-      <c r="F39" s="48"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="47"/>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="33">
+      <c r="D40" s="32">
         <v>27</v>
       </c>
-      <c r="E40" s="47"/>
-      <c r="F40" s="60"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="57"/>
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F41" s="88"/>
-      <c r="G41" s="88"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="12">
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Miscellaneous quality of life UI changes (state search merge lets you pick iter limit & max payload, load list building now assumes you dont need collision dependency config if you input invalid path)
</commit_message>
<xml_diff>
--- a/build files and notes/sheet w build methods info.xlsx
+++ b/build files and notes/sheet w build methods info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0044E48-BB6B-4DB7-8E94-D390E7C5E517}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F12405FF-DAA5-4D2E-89C8-4DE826C04F10}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
@@ -174,15 +174,9 @@
     <t>river</t>
   </si>
   <si>
-    <t>Payloads</t>
-  </si>
-  <si>
     <t>20, 19, 19, 18, 18</t>
   </si>
   <si>
-    <t>Occurence matrix (LL regeneration)</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
@@ -207,12 +201,6 @@
     <t>tested, works, no known lags</t>
   </si>
   <si>
-    <t>LL Gen. Settings</t>
-  </si>
-  <si>
-    <t>Occurence matrix   (no LL regeneration)</t>
-  </si>
-  <si>
     <t>22, 19, 19, 19, 19</t>
   </si>
   <si>
@@ -283,13 +271,25 @@
   </si>
   <si>
     <t>Xebra crash (mode 1/2)</t>
+  </si>
+  <si>
+    <t>24, 22, 22, 19, 19</t>
+  </si>
+  <si>
+    <t>Rel Occurence matrix   (no LL regeneration)</t>
+  </si>
+  <si>
+    <t>Abs Occurence matrix   (no LL regeneration)</t>
+  </si>
+  <si>
+    <t>22, 21, 21, 20, 19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,12 +333,6 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="238"/>
@@ -425,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -595,109 +589,18 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -705,22 +608,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -782,23 +676,11 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -815,124 +697,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -959,6 +727,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -968,13 +772,52 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1302,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AD2FBA-18F5-4705-80AA-981EA7CD31DD}">
-  <dimension ref="B1:I41"/>
+  <dimension ref="B1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1323,574 +1166,540 @@
   <sheetData>
     <row r="1" spans="2:9" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="50"/>
+    </row>
+    <row r="4" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="74"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="75" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="77"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="80"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="116"/>
-    </row>
-    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="60"/>
-    </row>
-    <row r="4" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="120" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="122"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="83" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="85"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="86" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="88"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="91"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="117" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="119"/>
+      <c r="B8" s="84" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="86"/>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="79" t="s">
+    <row r="11" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="87" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="92" t="s">
+      <c r="E11" s="94" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="91"/>
+      <c r="I11" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="88"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="I12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="96"/>
+      <c r="I13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="97" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="97" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="98"/>
+      <c r="I15" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="96"/>
+      <c r="I16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="I17" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="49">
+        <v>10</v>
+      </c>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="I18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="33">
+        <v>11</v>
+      </c>
+      <c r="E19" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="95"/>
-      <c r="I11" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="80"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="44" t="s">
+      <c r="F19" s="97"/>
+      <c r="I19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="39">
+        <v>12</v>
+      </c>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="I20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="33">
+        <v>13</v>
+      </c>
+      <c r="E21" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="99" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="48" t="s">
+      <c r="F21" s="97"/>
+      <c r="I21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="25">
+        <v>15</v>
+      </c>
+      <c r="E22" s="97"/>
+      <c r="F22" s="97"/>
+      <c r="I22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="40">
+        <v>16</v>
+      </c>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="I23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="25">
+        <v>17</v>
+      </c>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="I24" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="25">
+        <v>18</v>
+      </c>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="I25" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="37">
+        <v>19</v>
+      </c>
+      <c r="E26" s="97"/>
+      <c r="F26" s="97"/>
+      <c r="I26" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="99"/>
+      <c r="F27" s="99"/>
+    </row>
+    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
+    </row>
+    <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+    </row>
+    <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="97" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="97"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="96" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="96"/>
+    </row>
+    <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="7"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="99"/>
+    </row>
+    <row r="33" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="35">
+        <v>20</v>
+      </c>
+      <c r="E33" s="96"/>
+      <c r="F33" s="96"/>
+    </row>
+    <row r="34" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="35">
+        <v>21</v>
+      </c>
+      <c r="E34" s="96"/>
+      <c r="F34" s="96"/>
+    </row>
+    <row r="35" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="6">
+        <v>22</v>
+      </c>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
+    </row>
+    <row r="36" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="62"/>
-      <c r="G13" s="70"/>
-      <c r="I13" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="100" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="63"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="71"/>
-      <c r="I14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="98" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="70"/>
-      <c r="I15" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="112" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="96" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="59"/>
-      <c r="G16" s="72"/>
-      <c r="I16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="105" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="71"/>
-      <c r="I17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="104" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="56">
-        <v>10</v>
-      </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="71"/>
-      <c r="I18" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="111" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="36">
-        <v>11</v>
-      </c>
-      <c r="E19" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="71"/>
-      <c r="I19" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="108" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="42">
-        <v>12</v>
-      </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="71"/>
-      <c r="I20" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="111" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="36">
-        <v>13</v>
-      </c>
-      <c r="E21" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="71"/>
-      <c r="I21" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="106" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="18" t="s">
+      <c r="D36" s="24">
+        <v>23</v>
+      </c>
+      <c r="E36" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="97"/>
+    </row>
+    <row r="37" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="28">
-        <v>15</v>
-      </c>
-      <c r="E22" s="64"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="71"/>
-      <c r="I22" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="105" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="43">
-        <v>16</v>
-      </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="71"/>
-      <c r="I23" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="106" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="28">
-        <v>17</v>
-      </c>
-      <c r="E24" s="64"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="71"/>
-      <c r="I24" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="106" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="28">
-        <v>18</v>
-      </c>
-      <c r="E25" s="64"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="71"/>
-      <c r="I25" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="113" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="40">
-        <v>19</v>
-      </c>
-      <c r="E26" s="64"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="71"/>
-      <c r="I26" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="109" t="s">
+      <c r="D37" s="26">
         <v>24</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="65"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="73"/>
-    </row>
-    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="106" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="64"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="71"/>
-    </row>
-    <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="67"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="73"/>
-    </row>
-    <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="47"/>
-      <c r="G30" s="71"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="101" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="59"/>
-      <c r="G31" s="61"/>
-    </row>
-    <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="9"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="74"/>
-    </row>
-    <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="38">
-        <v>20</v>
-      </c>
-      <c r="E33" s="66"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="61"/>
-    </row>
-    <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="110" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="38">
-        <v>21</v>
-      </c>
-      <c r="E34" s="66"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="61"/>
-    </row>
-    <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="7">
-        <v>22</v>
-      </c>
-      <c r="E35" s="66"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="75"/>
-    </row>
-    <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="97" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="27">
-        <v>23</v>
-      </c>
-      <c r="E36" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="47"/>
-      <c r="G36" s="76"/>
-    </row>
-    <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="107" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="29">
-        <v>24</v>
-      </c>
-      <c r="E37" s="46"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="77"/>
-    </row>
-    <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E37" s="101"/>
+      <c r="F37" s="101"/>
+    </row>
+    <row r="38" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="22" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="4">
         <v>25</v>
       </c>
-      <c r="E38" s="58"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="103" t="s">
+      <c r="E38" s="102"/>
+      <c r="F38" s="102"/>
+    </row>
+    <row r="39" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="35">
+      <c r="D39" s="32">
         <v>26</v>
       </c>
-      <c r="E39" s="46"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="102" t="s">
+      <c r="E39" s="101"/>
+      <c r="F39" s="101"/>
+    </row>
+    <row r="40" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="32">
+      <c r="D40" s="29">
         <v>27</v>
       </c>
-      <c r="E40" s="46"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="11"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="101"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:G11"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
added new slightly random merge method based on waren's occurence matrix method that somehow is pretty good
</commit_message>
<xml_diff>
--- a/build files and notes/sheet w build methods info.xlsx
+++ b/build files and notes/sheet w build methods info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F12405FF-DAA5-4D2E-89C8-4DE826C04F10}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F12405FF-DAA5-4D2E-89C8-4DE826C04F10}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
+    <workbookView minimized="1" xWindow="15384" yWindow="4548" windowWidth="7656" windowHeight="4200" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
   <sheets>
     <sheet name="28.1. build test, ABS OCC" sheetId="2" r:id="rId1"/>
@@ -718,58 +718,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -784,9 +754,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,25 +766,58 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1148,7 +1148,7 @@
   <dimension ref="B1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,14 +1166,14 @@
   <sheetData>
     <row r="1" spans="2:9" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="71"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="51"/>
@@ -1184,85 +1184,85 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="74"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="90"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="77"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="93"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="80"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="96"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="83"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="99"/>
     </row>
     <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="86"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="102"/>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="89" t="s">
+      <c r="C11" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="94" t="s">
+      <c r="E11" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="94" t="s">
+      <c r="F11" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="91"/>
+      <c r="G11" s="69"/>
       <c r="I11" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="88"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
       <c r="I12" s="1" t="s">
         <v>60</v>
       </c>
@@ -1277,10 +1277,10 @@
       <c r="D13" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="96" t="s">
+      <c r="E13" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="96"/>
+      <c r="F13" s="70"/>
       <c r="I13" s="1" t="s">
         <v>61</v>
       </c>
@@ -1295,10 +1295,10 @@
       <c r="D14" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="97" t="s">
+      <c r="E14" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="97" t="s">
+      <c r="F14" s="71" t="s">
         <v>82</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1315,10 +1315,10 @@
       <c r="D15" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="98" t="s">
+      <c r="E15" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="98"/>
+      <c r="F15" s="72"/>
       <c r="I15" s="1" t="s">
         <v>63</v>
       </c>
@@ -1333,10 +1333,10 @@
       <c r="D16" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="96" t="s">
+      <c r="E16" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="96"/>
+      <c r="F16" s="70"/>
       <c r="I16" s="1" t="s">
         <v>64</v>
       </c>
@@ -1351,8 +1351,8 @@
       <c r="D17" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="97"/>
-      <c r="F17" s="97"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
       <c r="I17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1367,8 +1367,8 @@
       <c r="D18" s="49">
         <v>10</v>
       </c>
-      <c r="E18" s="97"/>
-      <c r="F18" s="97"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
       <c r="I18" s="1" t="s">
         <v>66</v>
       </c>
@@ -1383,10 +1383,10 @@
       <c r="D19" s="33">
         <v>11</v>
       </c>
-      <c r="E19" s="97" t="s">
+      <c r="E19" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="97"/>
+      <c r="F19" s="71"/>
       <c r="I19" s="1" t="s">
         <v>67</v>
       </c>
@@ -1401,8 +1401,8 @@
       <c r="D20" s="39">
         <v>12</v>
       </c>
-      <c r="E20" s="97"/>
-      <c r="F20" s="97"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
       <c r="I20" s="1" t="s">
         <v>68</v>
       </c>
@@ -1417,10 +1417,10 @@
       <c r="D21" s="33">
         <v>13</v>
       </c>
-      <c r="E21" s="97" t="s">
+      <c r="E21" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="97"/>
+      <c r="F21" s="71"/>
       <c r="I21" s="1" t="s">
         <v>69</v>
       </c>
@@ -1435,8 +1435,8 @@
       <c r="D22" s="25">
         <v>15</v>
       </c>
-      <c r="E22" s="97"/>
-      <c r="F22" s="97"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
       <c r="I22" s="1" t="s">
         <v>70</v>
       </c>
@@ -1451,8 +1451,8 @@
       <c r="D23" s="40">
         <v>16</v>
       </c>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
       <c r="I23" s="1" t="s">
         <v>71</v>
       </c>
@@ -1467,8 +1467,8 @@
       <c r="D24" s="25">
         <v>17</v>
       </c>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
       <c r="I24" s="1" t="s">
         <v>72</v>
       </c>
@@ -1483,8 +1483,8 @@
       <c r="D25" s="25">
         <v>18</v>
       </c>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
       <c r="I25" s="1" t="s">
         <v>73</v>
       </c>
@@ -1499,8 +1499,8 @@
       <c r="D26" s="37">
         <v>19</v>
       </c>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
       <c r="I26" s="1" t="s">
         <v>74</v>
       </c>
@@ -1515,8 +1515,8 @@
       <c r="D27" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="99"/>
-      <c r="F27" s="99"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
     </row>
     <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="61" t="s">
@@ -1528,8 +1528,8 @@
       <c r="D28" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="97"/>
-      <c r="F28" s="97"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
     </row>
     <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7" t="s">
@@ -1541,8 +1541,8 @@
       <c r="D29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="100"/>
-      <c r="F29" s="100"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
     </row>
     <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="55" t="s">
@@ -1554,10 +1554,10 @@
       <c r="D30" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="97" t="s">
+      <c r="E30" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="97"/>
+      <c r="F30" s="71"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="56" t="s">
@@ -1569,17 +1569,17 @@
       <c r="D31" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="96" t="s">
+      <c r="E31" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="96"/>
+      <c r="F31" s="70"/>
     </row>
     <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="7"/>
       <c r="C32" s="30"/>
       <c r="D32" s="31"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="99"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
     </row>
     <row r="33" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="65" t="s">
@@ -1591,8 +1591,8 @@
       <c r="D33" s="35">
         <v>20</v>
       </c>
-      <c r="E33" s="96"/>
-      <c r="F33" s="96"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
     </row>
     <row r="34" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="65" t="s">
@@ -1604,8 +1604,8 @@
       <c r="D34" s="35">
         <v>21</v>
       </c>
-      <c r="E34" s="96"/>
-      <c r="F34" s="96"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
     </row>
     <row r="35" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
@@ -1617,8 +1617,8 @@
       <c r="D35" s="6">
         <v>22</v>
       </c>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
     </row>
     <row r="36" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="52" t="s">
@@ -1630,10 +1630,10 @@
       <c r="D36" s="24">
         <v>23</v>
       </c>
-      <c r="E36" s="97" t="s">
+      <c r="E36" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="97"/>
+      <c r="F36" s="71"/>
     </row>
     <row r="37" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="62" t="s">
@@ -1645,8 +1645,8 @@
       <c r="D37" s="26">
         <v>24</v>
       </c>
-      <c r="E37" s="101"/>
-      <c r="F37" s="101"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
     </row>
     <row r="38" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
@@ -1658,8 +1658,8 @@
       <c r="D38" s="4">
         <v>25</v>
       </c>
-      <c r="E38" s="102"/>
-      <c r="F38" s="102"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="76"/>
     </row>
     <row r="39" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="58" t="s">
@@ -1671,8 +1671,8 @@
       <c r="D39" s="32">
         <v>26</v>
       </c>
-      <c r="E39" s="101"/>
-      <c r="F39" s="101"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
     </row>
     <row r="40" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="57" t="s">
@@ -1684,22 +1684,22 @@
       <c r="D40" s="29">
         <v>27</v>
       </c>
-      <c r="E40" s="101"/>
-      <c r="F40" s="101"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
improved the way method 4 picks the best merge it came up with, added some comments
</commit_message>
<xml_diff>
--- a/build files and notes/sheet w build methods info.xlsx
+++ b/build files and notes/sheet w build methods info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="429" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EE1C285-21C5-4E3A-A0A2-49FA64120960}"/>
+  <xr:revisionPtr revIDLastSave="432" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6CE44A9-01CA-44A4-9540-BF94D924B9A3}"/>
   <bookViews>
-    <workbookView xWindow="12156" yWindow="-108" windowWidth="7656" windowHeight="4200" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
+    <workbookView xWindow="12156" yWindow="0" windowWidth="7656" windowHeight="4200" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
   <sheets>
     <sheet name="All level build notes" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
   <si>
     <t>0A</t>
   </si>
@@ -271,12 +271,6 @@
   </si>
   <si>
     <t>Not playtested, assuming no lags</t>
-  </si>
-  <si>
-    <t>Yes perma, general dependency list, spawn 01_uZ, LL regen settings 5500/5500/5500/1/0.20, method 4 mult 1.5 seed 9827, built iter  2, max payload 21 (12_uZ)</t>
-  </si>
-  <si>
-    <t>Yes perma, general dependency list, spawn 01_cZ, LL regen settings 5500/5500/5500/1/0.25, method 4 mult 1.5 seed 21986, built iter 18, max payload 21 (35_cZ)</t>
   </si>
 </sst>
 </file>
@@ -532,113 +526,113 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -968,7 +962,7 @@
   <dimension ref="B3:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -982,13 +976,13 @@
   <sheetData>
     <row r="3" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="77" t="s">
         <v>76</v>
       </c>
       <c r="E4" s="41" t="s">
@@ -999,13 +993,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="77"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="78"/>
       <c r="E5" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="78"/>
+      <c r="F5" s="74"/>
     </row>
     <row r="6" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="26" t="s">
@@ -1014,13 +1008,13 @@
       <c r="C6" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="65"/>
+      <c r="F6" s="63"/>
     </row>
     <row r="7" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -1029,15 +1023,13 @@
       <c r="C7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="66" t="s">
-        <v>80</v>
-      </c>
+      <c r="F7" s="64"/>
     </row>
     <row r="8" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="25" t="s">
@@ -1046,13 +1038,13 @@
       <c r="C8" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="67" t="s">
+      <c r="E8" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="67"/>
+      <c r="F8" s="65"/>
     </row>
     <row r="9" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="39" t="s">
@@ -1061,13 +1053,13 @@
       <c r="C9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="69"/>
+      <c r="F9" s="67"/>
     </row>
     <row r="10" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="32" t="s">
@@ -1076,13 +1068,13 @@
       <c r="C10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="70"/>
+      <c r="F10" s="68"/>
     </row>
     <row r="11" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="31" t="s">
@@ -1091,13 +1083,13 @@
       <c r="C11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="48">
         <v>10</v>
       </c>
-      <c r="E11" s="73" t="s">
+      <c r="E11" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="73"/>
+      <c r="F11" s="71"/>
     </row>
     <row r="12" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="38" t="s">
@@ -1106,13 +1098,13 @@
       <c r="C12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="49">
         <v>11</v>
       </c>
-      <c r="E12" s="69" t="s">
+      <c r="E12" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="69"/>
+      <c r="F12" s="67"/>
     </row>
     <row r="13" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="35" t="s">
@@ -1121,13 +1113,13 @@
       <c r="C13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="52">
+      <c r="D13" s="50">
         <v>12</v>
       </c>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="72"/>
+      <c r="F13" s="70"/>
     </row>
     <row r="14" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="38" t="s">
@@ -1136,13 +1128,13 @@
       <c r="C14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="49">
         <v>13</v>
       </c>
-      <c r="E14" s="69" t="s">
+      <c r="E14" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="69"/>
+      <c r="F14" s="67"/>
     </row>
     <row r="15" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="33" t="s">
@@ -1151,13 +1143,13 @@
       <c r="C15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="53">
+      <c r="D15" s="51">
         <v>15</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="75"/>
+      <c r="F15" s="73"/>
     </row>
     <row r="16" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="32" t="s">
@@ -1166,13 +1158,13 @@
       <c r="C16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="49">
+      <c r="D16" s="47">
         <v>16</v>
       </c>
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="70"/>
+      <c r="F16" s="68"/>
     </row>
     <row r="17" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="33" t="s">
@@ -1181,13 +1173,13 @@
       <c r="C17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="53">
+      <c r="D17" s="51">
         <v>17</v>
       </c>
-      <c r="E17" s="75" t="s">
+      <c r="E17" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="75"/>
+      <c r="F17" s="73"/>
     </row>
     <row r="18" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="33" t="s">
@@ -1196,13 +1188,13 @@
       <c r="C18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="53">
+      <c r="D18" s="51">
         <v>18</v>
       </c>
-      <c r="E18" s="75" t="s">
+      <c r="E18" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="75"/>
+      <c r="F18" s="73"/>
     </row>
     <row r="19" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -1211,13 +1203,13 @@
       <c r="C19" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="52">
         <v>19</v>
       </c>
-      <c r="E19" s="71" t="s">
+      <c r="E19" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="71"/>
+      <c r="F19" s="69"/>
     </row>
     <row r="20" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="36" t="s">
@@ -1226,13 +1218,13 @@
       <c r="C20" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="72" t="s">
+      <c r="E20" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="72"/>
+      <c r="F20" s="70"/>
     </row>
     <row r="21" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="33" t="s">
@@ -1241,13 +1233,13 @@
       <c r="C21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="75" t="s">
+      <c r="E21" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="75"/>
+      <c r="F21" s="73"/>
     </row>
     <row r="22" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
@@ -1256,13 +1248,13 @@
       <c r="C22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="74" t="s">
+      <c r="E22" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="74"/>
+      <c r="F22" s="72"/>
     </row>
     <row r="23" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="27" t="s">
@@ -1271,15 +1263,13 @@
       <c r="C23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="66" t="s">
+      <c r="E23" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="66" t="s">
-        <v>79</v>
-      </c>
+      <c r="F23" s="64"/>
     </row>
     <row r="24" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="28" t="s">
@@ -1288,13 +1278,13 @@
       <c r="C24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="57" t="s">
+      <c r="D24" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="66" t="s">
+      <c r="E24" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="66"/>
+      <c r="F24" s="64"/>
     </row>
     <row r="25" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="37" t="s">
@@ -1303,13 +1293,13 @@
       <c r="C25" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="58">
+      <c r="D25" s="56">
         <v>20</v>
       </c>
-      <c r="E25" s="71" t="s">
+      <c r="E25" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="71"/>
+      <c r="F25" s="69"/>
     </row>
     <row r="26" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="37" t="s">
@@ -1318,13 +1308,13 @@
       <c r="C26" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="58">
+      <c r="D26" s="56">
         <v>21</v>
       </c>
-      <c r="E26" s="71" t="s">
+      <c r="E26" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="71"/>
+      <c r="F26" s="69"/>
     </row>
     <row r="27" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
@@ -1333,13 +1323,13 @@
       <c r="C27" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="59">
+      <c r="D27" s="57">
         <v>22</v>
       </c>
-      <c r="E27" s="74" t="s">
+      <c r="E27" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="74"/>
+      <c r="F27" s="72"/>
     </row>
     <row r="28" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="24" t="s">
@@ -1348,13 +1338,13 @@
       <c r="C28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="60">
+      <c r="D28" s="58">
         <v>23</v>
       </c>
-      <c r="E28" s="68" t="s">
+      <c r="E28" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="68"/>
+      <c r="F28" s="66"/>
     </row>
     <row r="29" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="34" t="s">
@@ -1363,13 +1353,13 @@
       <c r="C29" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="61">
+      <c r="D29" s="59">
         <v>24</v>
       </c>
-      <c r="E29" s="75" t="s">
+      <c r="E29" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="75"/>
+      <c r="F29" s="73"/>
     </row>
     <row r="30" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
@@ -1378,13 +1368,13 @@
       <c r="C30" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="62">
+      <c r="D30" s="60">
         <v>25</v>
       </c>
-      <c r="E30" s="74" t="s">
+      <c r="E30" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="74"/>
+      <c r="F30" s="72"/>
     </row>
     <row r="31" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="30" t="s">
@@ -1393,13 +1383,13 @@
       <c r="C31" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="63">
+      <c r="D31" s="61">
         <v>26</v>
       </c>
-      <c r="E31" s="73" t="s">
+      <c r="E31" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="73"/>
+      <c r="F31" s="71"/>
     </row>
     <row r="32" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="29" t="s">
@@ -1408,13 +1398,13 @@
       <c r="C32" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="64">
+      <c r="D32" s="62">
         <v>27</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>